<commit_message>
more THC initial implementation
-initial THC code implementation
-modified analog reading (AVR code)
</commit_message>
<xml_diff>
--- a/docs/avr_mcumap_gen.xlsx
+++ b/docs/avr_mcumap_gen.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uCNC-1.1.x\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCEM\Documents\GitHub\uCNC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7098BA7-8150-4B02-8ACD-AD787043EF8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EEC6B8-8362-494B-AE35-6A1C91109B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -7060,7 +7052,7 @@
       <c r="AA69" s="3"/>
       <c r="AB69" s="3"/>
     </row>
-    <row r="70" spans="1:28" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="4" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>67</v>
       </c>
@@ -7103,13 +7095,31 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="8" t="str">
-        <f>"#ifdef "&amp;C70&amp;"
+        <f>"#ifdef "&amp;C70&amp;"_CHANNEL
+#define "&amp;B70&amp;"_CHANNEL "&amp;C70&amp;"_CHANNEL
+#if("&amp;C70&amp;"_CHANNEL&lt;8)
+#define "&amp;B70&amp;"_MUX5 0x00
+#else
+#define "&amp;B70&amp;"_MUX5 0x04
+#endif
+#ifdef "&amp;C70&amp;"_PRESC
 #define "&amp;B70&amp;"_PRESC "&amp;C70&amp;"_PRESC
-#define  "&amp;B70&amp;"_CHANNEL "&amp;C70&amp;"_CHANNEL
+#else
+#define "&amp;B70&amp;"_PRESC 0
+#endif
 #endif"</f>
-        <v>#ifdef ANALOG0
+        <v>#ifdef ANALOG0_CHANNEL
+#define DIO67_CHANNEL ANALOG0_CHANNEL
+#if(ANALOG0_CHANNEL&lt;8)
+#define DIO67_MUX5 0x00
+#else
+#define DIO67_MUX5 0x04
+#endif
+#ifdef ANALOG0_PRESC
 #define DIO67_PRESC ANALOG0_PRESC
-#define  DIO67_CHANNEL ANALOG0_CHANNEL
+#else
+#define DIO67_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I70" s="3" t="str">
@@ -7172,13 +7182,31 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="8" t="str">
-        <f t="shared" ref="H71:H85" si="12">"#ifdef "&amp;C71&amp;"
+        <f t="shared" ref="H71:H85" si="12">"#ifdef "&amp;C71&amp;"_CHANNEL
+#define "&amp;B71&amp;"_CHANNEL "&amp;C71&amp;"_CHANNEL
+#if("&amp;C71&amp;"_CHANNEL&lt;8)
+#define "&amp;B71&amp;"_MUX5 0x00
+#else
+#define "&amp;B71&amp;"_MUX5 0x04
+#endif
+#ifdef "&amp;C71&amp;"_PRESC
 #define "&amp;B71&amp;"_PRESC "&amp;C71&amp;"_PRESC
-#define  "&amp;B71&amp;"_CHANNEL "&amp;C71&amp;"_CHANNEL
+#else
+#define "&amp;B71&amp;"_PRESC 0
+#endif
 #endif"</f>
-        <v>#ifdef ANALOG1
+        <v>#ifdef ANALOG1_CHANNEL
+#define DIO68_CHANNEL ANALOG1_CHANNEL
+#if(ANALOG1_CHANNEL&lt;8)
+#define DIO68_MUX5 0x00
+#else
+#define DIO68_MUX5 0x04
+#endif
+#ifdef ANALOG1_PRESC
 #define DIO68_PRESC ANALOG1_PRESC
-#define  DIO68_CHANNEL ANALOG1_CHANNEL
+#else
+#define DIO68_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I71" s="3" t="str">
@@ -7242,9 +7270,18 @@
       <c r="G72" s="6"/>
       <c r="H72" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG2
+        <v>#ifdef ANALOG2_CHANNEL
+#define DIO69_CHANNEL ANALOG2_CHANNEL
+#if(ANALOG2_CHANNEL&lt;8)
+#define DIO69_MUX5 0x00
+#else
+#define DIO69_MUX5 0x04
+#endif
+#ifdef ANALOG2_PRESC
 #define DIO69_PRESC ANALOG2_PRESC
-#define  DIO69_CHANNEL ANALOG2_CHANNEL
+#else
+#define DIO69_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I72" s="3" t="str">
@@ -7306,9 +7343,18 @@
       <c r="G73" s="6"/>
       <c r="H73" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG3
+        <v>#ifdef ANALOG3_CHANNEL
+#define DIO70_CHANNEL ANALOG3_CHANNEL
+#if(ANALOG3_CHANNEL&lt;8)
+#define DIO70_MUX5 0x00
+#else
+#define DIO70_MUX5 0x04
+#endif
+#ifdef ANALOG3_PRESC
 #define DIO70_PRESC ANALOG3_PRESC
-#define  DIO70_CHANNEL ANALOG3_CHANNEL
+#else
+#define DIO70_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I73" s="3" t="str">
@@ -7370,9 +7416,18 @@
       <c r="G74" s="6"/>
       <c r="H74" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG4
+        <v>#ifdef ANALOG4_CHANNEL
+#define DIO71_CHANNEL ANALOG4_CHANNEL
+#if(ANALOG4_CHANNEL&lt;8)
+#define DIO71_MUX5 0x00
+#else
+#define DIO71_MUX5 0x04
+#endif
+#ifdef ANALOG4_PRESC
 #define DIO71_PRESC ANALOG4_PRESC
-#define  DIO71_CHANNEL ANALOG4_CHANNEL
+#else
+#define DIO71_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I74" s="3" t="str">
@@ -7434,9 +7489,18 @@
       <c r="G75" s="6"/>
       <c r="H75" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG5
+        <v>#ifdef ANALOG5_CHANNEL
+#define DIO72_CHANNEL ANALOG5_CHANNEL
+#if(ANALOG5_CHANNEL&lt;8)
+#define DIO72_MUX5 0x00
+#else
+#define DIO72_MUX5 0x04
+#endif
+#ifdef ANALOG5_PRESC
 #define DIO72_PRESC ANALOG5_PRESC
-#define  DIO72_CHANNEL ANALOG5_CHANNEL
+#else
+#define DIO72_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I75" s="3" t="str">
@@ -7498,9 +7562,18 @@
       <c r="G76" s="6"/>
       <c r="H76" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG6
+        <v>#ifdef ANALOG6_CHANNEL
+#define DIO73_CHANNEL ANALOG6_CHANNEL
+#if(ANALOG6_CHANNEL&lt;8)
+#define DIO73_MUX5 0x00
+#else
+#define DIO73_MUX5 0x04
+#endif
+#ifdef ANALOG6_PRESC
 #define DIO73_PRESC ANALOG6_PRESC
-#define  DIO73_CHANNEL ANALOG6_CHANNEL
+#else
+#define DIO73_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I76" s="3" t="str">
@@ -7562,9 +7635,18 @@
       <c r="G77" s="6"/>
       <c r="H77" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG7
+        <v>#ifdef ANALOG7_CHANNEL
+#define DIO74_CHANNEL ANALOG7_CHANNEL
+#if(ANALOG7_CHANNEL&lt;8)
+#define DIO74_MUX5 0x00
+#else
+#define DIO74_MUX5 0x04
+#endif
+#ifdef ANALOG7_PRESC
 #define DIO74_PRESC ANALOG7_PRESC
-#define  DIO74_CHANNEL ANALOG7_CHANNEL
+#else
+#define DIO74_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I77" s="3" t="str">
@@ -7626,9 +7708,18 @@
       <c r="G78" s="6"/>
       <c r="H78" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG8
+        <v>#ifdef ANALOG8_CHANNEL
+#define DIO75_CHANNEL ANALOG8_CHANNEL
+#if(ANALOG8_CHANNEL&lt;8)
+#define DIO75_MUX5 0x00
+#else
+#define DIO75_MUX5 0x04
+#endif
+#ifdef ANALOG8_PRESC
 #define DIO75_PRESC ANALOG8_PRESC
-#define  DIO75_CHANNEL ANALOG8_CHANNEL
+#else
+#define DIO75_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I78" s="3" t="str">
@@ -7690,9 +7781,18 @@
       <c r="G79" s="6"/>
       <c r="H79" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG9
+        <v>#ifdef ANALOG9_CHANNEL
+#define DIO76_CHANNEL ANALOG9_CHANNEL
+#if(ANALOG9_CHANNEL&lt;8)
+#define DIO76_MUX5 0x00
+#else
+#define DIO76_MUX5 0x04
+#endif
+#ifdef ANALOG9_PRESC
 #define DIO76_PRESC ANALOG9_PRESC
-#define  DIO76_CHANNEL ANALOG9_CHANNEL
+#else
+#define DIO76_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I79" s="3" t="str">
@@ -7754,9 +7854,18 @@
       <c r="G80" s="6"/>
       <c r="H80" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG10
+        <v>#ifdef ANALOG10_CHANNEL
+#define DIO77_CHANNEL ANALOG10_CHANNEL
+#if(ANALOG10_CHANNEL&lt;8)
+#define DIO77_MUX5 0x00
+#else
+#define DIO77_MUX5 0x04
+#endif
+#ifdef ANALOG10_PRESC
 #define DIO77_PRESC ANALOG10_PRESC
-#define  DIO77_CHANNEL ANALOG10_CHANNEL
+#else
+#define DIO77_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I80" s="3" t="str">
@@ -7818,9 +7927,18 @@
       <c r="G81" s="6"/>
       <c r="H81" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG11
+        <v>#ifdef ANALOG11_CHANNEL
+#define DIO78_CHANNEL ANALOG11_CHANNEL
+#if(ANALOG11_CHANNEL&lt;8)
+#define DIO78_MUX5 0x00
+#else
+#define DIO78_MUX5 0x04
+#endif
+#ifdef ANALOG11_PRESC
 #define DIO78_PRESC ANALOG11_PRESC
-#define  DIO78_CHANNEL ANALOG11_CHANNEL
+#else
+#define DIO78_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I81" s="3" t="str">
@@ -7882,9 +8000,18 @@
       <c r="G82" s="6"/>
       <c r="H82" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG12
+        <v>#ifdef ANALOG12_CHANNEL
+#define DIO79_CHANNEL ANALOG12_CHANNEL
+#if(ANALOG12_CHANNEL&lt;8)
+#define DIO79_MUX5 0x00
+#else
+#define DIO79_MUX5 0x04
+#endif
+#ifdef ANALOG12_PRESC
 #define DIO79_PRESC ANALOG12_PRESC
-#define  DIO79_CHANNEL ANALOG12_CHANNEL
+#else
+#define DIO79_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I82" s="3" t="str">
@@ -7946,9 +8073,18 @@
       <c r="G83" s="6"/>
       <c r="H83" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG13
+        <v>#ifdef ANALOG13_CHANNEL
+#define DIO80_CHANNEL ANALOG13_CHANNEL
+#if(ANALOG13_CHANNEL&lt;8)
+#define DIO80_MUX5 0x00
+#else
+#define DIO80_MUX5 0x04
+#endif
+#ifdef ANALOG13_PRESC
 #define DIO80_PRESC ANALOG13_PRESC
-#define  DIO80_CHANNEL ANALOG13_CHANNEL
+#else
+#define DIO80_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I83" s="3" t="str">
@@ -8010,9 +8146,18 @@
       <c r="G84" s="6"/>
       <c r="H84" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG14
+        <v>#ifdef ANALOG14_CHANNEL
+#define DIO81_CHANNEL ANALOG14_CHANNEL
+#if(ANALOG14_CHANNEL&lt;8)
+#define DIO81_MUX5 0x00
+#else
+#define DIO81_MUX5 0x04
+#endif
+#ifdef ANALOG14_PRESC
 #define DIO81_PRESC ANALOG14_PRESC
-#define  DIO81_CHANNEL ANALOG14_CHANNEL
+#else
+#define DIO81_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I84" s="3" t="str">
@@ -8074,9 +8219,18 @@
       <c r="G85" s="6"/>
       <c r="H85" s="8" t="str">
         <f t="shared" si="12"/>
-        <v>#ifdef ANALOG15
+        <v>#ifdef ANALOG15_CHANNEL
+#define DIO82_CHANNEL ANALOG15_CHANNEL
+#if(ANALOG15_CHANNEL&lt;8)
+#define DIO82_MUX5 0x00
+#else
+#define DIO82_MUX5 0x04
+#endif
+#ifdef ANALOG15_PRESC
 #define DIO82_PRESC ANALOG15_PRESC
-#define  DIO82_CHANNEL ANALOG15_CHANNEL
+#else
+#define DIO82_PRESC 0
+#endif
 #endif</v>
       </c>
       <c r="I85" s="3" t="str">

</xml_diff>